<commit_message>
Fix wifi, update setup guide, output MVNC graph file
</commit_message>
<xml_diff>
--- a/Thesis Project - Gantt Chart.xlsx
+++ b/Thesis Project - Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\EEE4022S - thesis project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\EEE4022S Thesis Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B5E577-B8E0-40BE-9C3E-0D27FA06BF41}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD70511-431A-4A0C-B69C-92962BE8DF8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8860" xr2:uid="{A2B2673A-199A-4790-994A-444B0E0296E2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="27">
   <si>
     <t>T</t>
   </si>
@@ -58,17 +58,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Hardware setup:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Rpi + put NN onto NCS</t>
+      <t>Basic tracking algorithm:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> proportional (+ integrate?)</t>
     </r>
   </si>
   <si>
@@ -81,17 +81,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Basic tracking algorithm:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> proportional (+ integrate?)</t>
+      <t>Kalman filter:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> understand + implement</t>
     </r>
   </si>
   <si>
@@ -104,17 +104,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Kalman filter:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> understand + implement</t>
+      <t>Planning + revision:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of project + previous work</t>
     </r>
   </si>
   <si>
@@ -127,17 +127,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Planning + revision:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of project + previous work</t>
+      <t>Create NN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> recognise dogs + draw a box around em</t>
     </r>
   </si>
   <si>
@@ -150,17 +150,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Create NN:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> recognise dogs + draw a box around em</t>
+      <t>Data:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> collect + label photos + videos of dogs</t>
     </r>
   </si>
   <si>
@@ -173,17 +173,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Data:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> collect + label photos + videos of dogs</t>
+      <t>Convert to cheetah tracker:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> collect + label new data</t>
     </r>
   </si>
   <si>
@@ -196,17 +196,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Convert to cheetah tracker:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> collect + label new data</t>
+      <t>Camera gimbal:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> design + 3D print</t>
     </r>
   </si>
   <si>
@@ -219,18 +219,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Camera gimbal:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> design + 3D print</t>
-    </r>
+      <t>Write up thesis:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do it in LaTeX</t>
+    </r>
+  </si>
+  <si>
+    <t>60p high</t>
   </si>
   <si>
     <r>
@@ -242,24 +245,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Write up thesis:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> do it in LaTeX</t>
-    </r>
-  </si>
-  <si>
-    <t>60p high</t>
-  </si>
-  <si>
-    <t>EXTRA</t>
+      <t>Improve control algorithm:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> make it track pan + tilt</t>
+    </r>
   </si>
   <si>
     <r>
@@ -271,18 +268,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Improve control algorithm:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> make it track pan + tilt</t>
-    </r>
+      <t>Hardware test:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> put NN onto NCS, test entire system</t>
+    </r>
+  </si>
+  <si>
+    <t>holding off on any planning from this point on until I have a better</t>
+  </si>
+  <si>
+    <t>idea of how busy I'll be during the semester/when tests + projects</t>
+  </si>
+  <si>
+    <t>are due these are just preliminary estimates to get an idea of how</t>
   </si>
   <si>
     <r>
@@ -294,18 +300,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Hardware test:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> put NN onto NCS, test entire system</t>
-    </r>
+      <t>Convert to cheetah tracker 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: tweak NN architecture</t>
+    </r>
+  </si>
+  <si>
+    <t>much time I'll have for things (eg one block is about 8 hours of</t>
+  </si>
+  <si>
+    <t>work now, but will be less during 3rd quarter and more in 4th)</t>
   </si>
   <si>
     <r>
@@ -317,6 +329,55 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Rig setup:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> set up the minibeast for NN training</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Set up pi:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> everything got mangled -&gt; reinstall</t>
+    </r>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/openimages/web/download.html    ???</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Educate:</t>
     </r>
     <r>
@@ -327,7 +388,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> watch fast.ai part 2 and read papers</t>
+      <t xml:space="preserve"> watch fast.ai part 2, read papers and blogs</t>
     </r>
   </si>
 </sst>
@@ -335,7 +396,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +415,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,10 +492,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,6 +517,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -456,11 +530,9 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -773,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95E18EA-BCFA-4AAA-B598-899C1821AABC}">
-  <dimension ref="A1:CN29"/>
+  <dimension ref="A1:CN32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,160 +861,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="12">
         <v>43276</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12">
         <v>43283</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10">
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12">
         <v>43290</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10">
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12">
         <v>43297</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10">
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12">
         <v>43304</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10">
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12">
         <v>43311</v>
       </c>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10">
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12">
         <v>43318</v>
       </c>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10">
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12">
         <v>43325</v>
       </c>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10">
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12">
         <v>43332</v>
       </c>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10">
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12">
         <v>43339</v>
       </c>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="10"/>
-      <c r="AZ1" s="10">
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12">
         <v>43346</v>
       </c>
-      <c r="BA1" s="10"/>
-      <c r="BB1" s="10"/>
-      <c r="BC1" s="10"/>
-      <c r="BD1" s="10"/>
-      <c r="BE1" s="10">
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12">
         <v>43353</v>
       </c>
-      <c r="BF1" s="10"/>
-      <c r="BG1" s="10"/>
-      <c r="BH1" s="10"/>
-      <c r="BI1" s="10"/>
-      <c r="BJ1" s="10">
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12">
         <v>43360</v>
       </c>
-      <c r="BK1" s="10"/>
-      <c r="BL1" s="10"/>
-      <c r="BM1" s="10"/>
-      <c r="BN1" s="10"/>
-      <c r="BO1" s="10">
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12">
         <v>43367</v>
       </c>
-      <c r="BP1" s="10"/>
-      <c r="BQ1" s="10"/>
-      <c r="BR1" s="10"/>
-      <c r="BS1" s="10"/>
-      <c r="BT1" s="10">
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BR1" s="12"/>
+      <c r="BS1" s="12"/>
+      <c r="BT1" s="12">
         <v>43374</v>
       </c>
-      <c r="BU1" s="10"/>
-      <c r="BV1" s="10"/>
-      <c r="BW1" s="10"/>
-      <c r="BX1" s="10"/>
-      <c r="BY1" s="10">
+      <c r="BU1" s="12"/>
+      <c r="BV1" s="12"/>
+      <c r="BW1" s="12"/>
+      <c r="BX1" s="12"/>
+      <c r="BY1" s="12">
         <v>43381</v>
       </c>
-      <c r="BZ1" s="10"/>
-      <c r="CA1" s="10"/>
-      <c r="CB1" s="10"/>
-      <c r="CC1" s="10"/>
-      <c r="CD1" s="10">
+      <c r="BZ1" s="12"/>
+      <c r="CA1" s="12"/>
+      <c r="CB1" s="12"/>
+      <c r="CC1" s="12"/>
+      <c r="CD1" s="12">
         <v>43388</v>
       </c>
-      <c r="CE1" s="10"/>
-      <c r="CF1" s="10"/>
-      <c r="CG1" s="10"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="10">
+      <c r="CE1" s="12"/>
+      <c r="CF1" s="12"/>
+      <c r="CG1" s="12"/>
+      <c r="CH1" s="14"/>
+      <c r="CI1" s="12">
         <v>43389</v>
       </c>
-      <c r="CJ1" s="10"/>
-      <c r="CK1" s="10"/>
-      <c r="CL1" s="10"/>
-      <c r="CM1" s="12"/>
+      <c r="CJ1" s="12"/>
+      <c r="CK1" s="12"/>
+      <c r="CL1" s="12"/>
+      <c r="CM1" s="14"/>
     </row>
     <row r="2" spans="1:92" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="5" t="s">
@@ -1197,136 +1269,187 @@
     </row>
     <row r="3" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="CN3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:92" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>26</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
+      <c r="I4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:92" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:92" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-    </row>
-    <row r="10" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>9</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="9"/>
+    </row>
     <row r="11" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
-      <c r="AJ11" s="3"/>
-      <c r="AK11" s="3"/>
-      <c r="AL11" s="3"/>
-    </row>
-    <row r="12" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AM12" s="3"/>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="3"/>
-    </row>
+        <v>6</v>
+      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+    </row>
+    <row r="12" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS13" s="3"/>
-      <c r="AT13" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
     </row>
     <row r="14" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BO14" s="3"/>
-      <c r="BP14" s="3"/>
-      <c r="BQ14" s="3"/>
-      <c r="BR14" s="3"/>
-      <c r="BS14" s="3"/>
-      <c r="BT14" s="3"/>
-      <c r="BU14" s="3"/>
-      <c r="BV14" s="3"/>
-      <c r="BW14" s="3"/>
-      <c r="BX14" s="3"/>
-      <c r="BY14" s="3"/>
-      <c r="BZ14" s="3"/>
-      <c r="CA14" s="3"/>
-      <c r="CB14" s="3"/>
-      <c r="CC14" s="3"/>
-    </row>
-    <row r="15" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+    </row>
+    <row r="15" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AQ15" s="3"/>
+      <c r="AR15" s="3"/>
+    </row>
+    <row r="16" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AR16" s="4"/>
+      <c r="AS16" s="3"/>
+      <c r="AT16" s="3"/>
+      <c r="AU16" s="3"/>
+    </row>
+    <row r="17" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="BO17" s="3"/>
+      <c r="BP17" s="3"/>
+      <c r="BQ17" s="3"/>
+      <c r="BR17" s="3"/>
+      <c r="BS17" s="3"/>
+      <c r="BT17" s="3"/>
+      <c r="BU17" s="3"/>
+      <c r="BV17" s="3"/>
+      <c r="BW17" s="3"/>
+      <c r="BX17" s="3"/>
+      <c r="BY17" s="3"/>
+      <c r="BZ17" s="3"/>
+      <c r="CA17" s="3"/>
+      <c r="CB17" s="3"/>
+      <c r="CC17" s="3"/>
+    </row>
+    <row r="18" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="BY1:CC1"/>
@@ -1349,7 +1472,10 @@
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="V1:Z1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AP15" r:id="rId1" xr:uid="{8107936F-93B0-4614-992A-90AE0C6EAA36}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add tex docs, notebooks, start of main code
</commit_message>
<xml_diff>
--- a/Thesis Project - Gantt Chart.xlsx
+++ b/Thesis Project - Gantt Chart.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\EEE4022S Thesis Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4DBF69-13A4-477C-902E-A73324F16B97}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8C057-16FD-4F46-8E32-519A43A4D032}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8860" xr2:uid="{A2B2673A-199A-4790-994A-444B0E0296E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (old)" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Display_Week" localSheetId="1">'Sheet1 (old)'!#REF!</definedName>
     <definedName name="Display_Week">Sheet1!#REF!</definedName>
+    <definedName name="Project_Start" localSheetId="1">'Sheet1 (old)'!#REF!</definedName>
     <definedName name="Project_Start">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="28">
   <si>
     <t>T</t>
   </si>
@@ -58,29 +61,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Basic tracking algorithm:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> proportional (+ integrate?)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Planning + revision:</t>
     </r>
     <r>
@@ -107,17 +87,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Improve control algorithm:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> make it track pan + tilt</t>
+      <t>Set up pi:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> everything got mangled -&gt; reinstall</t>
     </r>
   </si>
   <si>
@@ -130,17 +110,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Set up pi:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> everything got mangled -&gt; reinstall</t>
+      <t>Educate:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> watch fast.ai part 2, read papers and blogs</t>
     </r>
   </si>
   <si>
@@ -153,17 +133,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Educate:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> watch fast.ai part 2, read papers and blogs</t>
+      <t>Set up minibeast:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> install python, tensorflow, etc</t>
     </r>
   </si>
   <si>
@@ -176,17 +156,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Set up minibeast:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> install python, tensorflow, etc</t>
+      <t>Hardware test:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> compile NN into graph, put on NCS</t>
     </r>
   </si>
   <si>
@@ -199,17 +179,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Hardware test:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> compile NN into graph, put on NCS</t>
+      <t>Camera gimbal:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> design, 3D print, put together</t>
     </r>
   </si>
   <si>
@@ -222,29 +202,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Camera gimbal:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> design, 3D print, put together</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Extended Kalman Filter:</t>
     </r>
     <r>
@@ -256,29 +213,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> understand + implement</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Convert to dog tracker:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> get data, train</t>
     </r>
   </si>
   <si>
@@ -466,6 +400,121 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> switch to tf, finetune model, compile</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Work on control:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> make it track pan + tilt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Work on "extras":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> eg put on quad, etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Integration time:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> put everything together, test</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Camera gimbal 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fetch, print frame, assemble, test</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Camera gimbal:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> compare options, order</t>
     </r>
   </si>
 </sst>
@@ -473,7 +522,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,20 +541,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -575,11 +610,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -607,7 +641,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,11 +656,17 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -638,12 +677,11 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -956,11 +994,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95E18EA-BCFA-4AAA-B598-899C1821AABC}">
-  <dimension ref="A1:CX34"/>
+  <dimension ref="A1:CT34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AS10" sqref="AS10"/>
+      <pane xSplit="1" topLeftCell="BF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BG14" sqref="BG14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -968,157 +1006,149 @@
     <col min="1" max="1" width="23.6328125" style="2" customWidth="1"/>
     <col min="2" max="20" width="2.81640625" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="2.81640625" style="7" hidden="1" customWidth="1"/>
-    <col min="22" max="28" width="2.81640625" hidden="1" customWidth="1"/>
-    <col min="29" max="44" width="2.81640625" customWidth="1"/>
-    <col min="45" max="47" width="2.7265625" customWidth="1"/>
-    <col min="48" max="49" width="2.81640625" customWidth="1"/>
-    <col min="50" max="54" width="2.7265625" customWidth="1"/>
-    <col min="55" max="56" width="2.81640625" customWidth="1"/>
-    <col min="57" max="101" width="2.7265625" customWidth="1"/>
+    <col min="22" max="44" width="2.81640625" hidden="1" customWidth="1"/>
+    <col min="45" max="57" width="2.7265625" hidden="1" customWidth="1"/>
+    <col min="58" max="97" width="2.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="21">
+      <c r="B1" s="22">
         <v>43276</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22">
         <v>43283</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21">
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22">
         <v>43290</v>
       </c>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21">
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22">
         <v>43297</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22">
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23">
         <v>43304</v>
       </c>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="23">
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="24">
         <v>43311</v>
       </c>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="23">
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="24">
         <v>43318</v>
       </c>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="17"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="16"/>
       <c r="AQ1" s="23">
         <v>43325</v>
       </c>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="23">
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="24">
         <v>43332</v>
       </c>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="21">
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="22">
         <v>43339</v>
       </c>
-      <c r="BF1" s="21"/>
-      <c r="BG1" s="21"/>
-      <c r="BH1" s="21"/>
-      <c r="BI1" s="21"/>
-      <c r="BJ1" s="21">
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22">
         <v>43346</v>
       </c>
-      <c r="BK1" s="21"/>
-      <c r="BL1" s="21"/>
-      <c r="BM1" s="21"/>
-      <c r="BN1" s="21"/>
-      <c r="BO1" s="21">
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22">
         <v>43353</v>
       </c>
-      <c r="BP1" s="21"/>
-      <c r="BQ1" s="21"/>
-      <c r="BR1" s="21"/>
-      <c r="BS1" s="21"/>
-      <c r="BT1" s="21">
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22">
         <v>43360</v>
       </c>
-      <c r="BU1" s="21"/>
-      <c r="BV1" s="21"/>
-      <c r="BW1" s="21"/>
-      <c r="BX1" s="21"/>
-      <c r="BY1" s="21">
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22">
         <v>43367</v>
       </c>
-      <c r="BZ1" s="21"/>
-      <c r="CA1" s="21"/>
-      <c r="CB1" s="21"/>
-      <c r="CC1" s="21"/>
-      <c r="CD1" s="21">
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22">
         <v>43374</v>
       </c>
-      <c r="CE1" s="21"/>
-      <c r="CF1" s="21"/>
-      <c r="CG1" s="21"/>
-      <c r="CH1" s="21"/>
-      <c r="CI1" s="21">
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
+      <c r="CC1" s="22"/>
+      <c r="CD1" s="22"/>
+      <c r="CE1" s="22">
         <v>43381</v>
       </c>
-      <c r="CJ1" s="21"/>
-      <c r="CK1" s="21"/>
-      <c r="CL1" s="21"/>
-      <c r="CM1" s="21"/>
-      <c r="CN1" s="21">
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22">
         <v>43388</v>
       </c>
-      <c r="CO1" s="21"/>
-      <c r="CP1" s="21"/>
-      <c r="CQ1" s="21"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="23"/>
+      <c r="CO1" s="22">
+        <v>43395</v>
+      </c>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
       <c r="CR1" s="22"/>
-      <c r="CS1" s="21">
-        <v>43395</v>
-      </c>
-      <c r="CT1" s="21"/>
-      <c r="CU1" s="21"/>
-      <c r="CV1" s="21"/>
-      <c r="CW1" s="22"/>
-    </row>
-    <row r="2" spans="1:102" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="CS1" s="23"/>
+    </row>
+    <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="9" t="s">
         <v>3</v>
@@ -1177,7 +1207,7 @@
       <c r="T2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V2" s="9" t="s">
@@ -1196,12 +1226,12 @@
         <v>2</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="AD2" s="9" t="s">
@@ -1217,10 +1247,10 @@
         <v>2</v>
       </c>
       <c r="AH2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AI2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>3</v>
@@ -1238,206 +1268,194 @@
         <v>2</v>
       </c>
       <c r="AO2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AP2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AQ2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AR2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AR2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="AU2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AV2" s="19" t="s">
-        <v>20</v>
+      <c r="AV2" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="AW2" s="5" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AX2" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AY2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="AZ2" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC2" s="19" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="BC2" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="BD2" s="5" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BE2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BF2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH2" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BJ2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BK2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM2" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BO2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BP2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BQ2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR2" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BT2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BU2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BV2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW2" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BY2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BZ2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CA2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB2" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="CD2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="CE2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CF2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG2" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="CI2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="CJ2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CK2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL2" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="CN2" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="CN2" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="CO2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CP2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CQ2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="CR2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CS2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="CT2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="CU2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="CV2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="CW2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CX2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CR2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CS2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CT2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:102" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="CX3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:102" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CT3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1448,9 +1466,9 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:102" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1474,9 +1492,9 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:102" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1499,9 +1517,9 @@
       <c r="U6" s="8"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:102" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1523,9 +1541,9 @@
       <c r="V7" s="3"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:102" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4"/>
       <c r="G8" s="4"/>
@@ -1556,14 +1574,10 @@
       <c r="AI8" s="4"/>
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
-      <c r="AV8" s="4"/>
-      <c r="AW8" s="4"/>
-      <c r="BC8" s="4"/>
-      <c r="BD8" s="4"/>
-    </row>
-    <row r="9" spans="1:102" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4"/>
       <c r="G9" s="4"/>
@@ -1602,14 +1616,10 @@
       <c r="AN9" s="4"/>
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
-      <c r="AV9" s="4"/>
-      <c r="AW9" s="4"/>
-      <c r="BC9" s="4"/>
-      <c r="BD9" s="4"/>
-    </row>
-    <row r="10" spans="1:102" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
-        <v>25</v>
+    </row>
+    <row r="10" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D10" s="4"/>
       <c r="G10" s="4"/>
@@ -1651,14 +1661,10 @@
       <c r="AQ10" s="3"/>
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
-      <c r="AV10" s="4"/>
-      <c r="AW10" s="4"/>
-      <c r="BC10" s="4"/>
-      <c r="BD10" s="4"/>
-    </row>
-    <row r="11" spans="1:102" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4"/>
       <c r="G11" s="4"/>
@@ -1689,12 +1695,10 @@
       <c r="AF11" s="4"/>
       <c r="AO11" s="4"/>
       <c r="AS11" s="3"/>
-      <c r="AV11" s="4"/>
-      <c r="BC11" s="4"/>
-    </row>
-    <row r="12" spans="1:102" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1731,14 +1735,15 @@
       <c r="AR12" s="4"/>
       <c r="AT12" s="3"/>
       <c r="AU12" s="3"/>
-      <c r="AV12" s="4"/>
-      <c r="AW12" s="4"/>
-      <c r="BC12" s="4"/>
-      <c r="BD12" s="4"/>
-    </row>
-    <row r="13" spans="1:102" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AV12" s="3"/>
+      <c r="AW12" s="3"/>
+      <c r="AX12" s="3"/>
+      <c r="AY12" s="3"/>
+      <c r="AZ12" s="3"/>
+    </row>
+    <row r="13" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1758,13 +1763,38 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
-      <c r="AX13" s="3"/>
-      <c r="AY13" s="3"/>
-      <c r="AZ13" s="3"/>
-    </row>
-    <row r="14" spans="1:102" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="4"/>
+      <c r="AO13" s="4"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AT13" s="3"/>
+      <c r="AU13" s="3"/>
+      <c r="BA13" s="3"/>
+      <c r="BB13" s="3"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
+      <c r="BG13" s="3"/>
+      <c r="BH13" s="3"/>
+      <c r="BI13" s="3"/>
+      <c r="BJ13" s="3"/>
+      <c r="BK13" s="3"/>
+    </row>
+    <row r="14" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1784,15 +1814,13 @@
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
-      <c r="AX14" s="3"/>
-      <c r="AY14" s="3"/>
-      <c r="AZ14" s="3"/>
-      <c r="BA14" s="3"/>
-      <c r="BB14" s="3"/>
-    </row>
-    <row r="15" spans="1:102" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
+      <c r="BJ14" s="3"/>
+    </row>
+    <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1812,15 +1840,14 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
-      <c r="BE15" s="3"/>
-      <c r="BF15" s="3"/>
-      <c r="BG15" s="3"/>
-      <c r="BH15" s="3"/>
-      <c r="BI15" s="3"/>
-    </row>
-    <row r="16" spans="1:102" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BK15" s="3"/>
+      <c r="BL15" s="3"/>
+      <c r="BM15" s="3"/>
+      <c r="BN15" s="3"/>
+    </row>
+    <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AG16" s="4"/>
       <c r="AJ16" s="4"/>
@@ -1833,25 +1860,25 @@
       <c r="AS16" s="4"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
+      <c r="AV16" s="4"/>
+      <c r="AW16" s="4"/>
       <c r="AX16" s="4"/>
       <c r="AY16" s="4"/>
       <c r="AZ16" s="4"/>
-      <c r="BA16" s="4"/>
-      <c r="BB16" s="4"/>
-      <c r="BE16" s="4"/>
       <c r="BF16" s="4"/>
       <c r="BG16" s="4"/>
       <c r="BH16" s="4"/>
       <c r="BI16" s="4"/>
-      <c r="BJ16" s="3"/>
-      <c r="BK16" s="3"/>
-      <c r="BL16" s="3"/>
-      <c r="BM16" s="3"/>
+      <c r="BJ16" s="4"/>
+      <c r="BK16" s="4"/>
+      <c r="BL16" s="4"/>
+      <c r="BM16" s="4"/>
       <c r="BN16" s="3"/>
-    </row>
-    <row r="17" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BO16" s="3"/>
+    </row>
+    <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AG17" s="4"/>
       <c r="AJ17" s="4"/>
@@ -1864,26 +1891,23 @@
       <c r="AS17" s="4"/>
       <c r="AT17" s="4"/>
       <c r="AU17" s="4"/>
-      <c r="AX17" s="13"/>
+      <c r="AV17" s="4"/>
+      <c r="AW17" s="4"/>
+      <c r="AX17" s="4"/>
       <c r="AY17" s="4"/>
       <c r="AZ17" s="4"/>
-      <c r="BA17" s="4"/>
-      <c r="BB17" s="4"/>
-      <c r="BE17" s="4"/>
       <c r="BF17" s="4"/>
       <c r="BG17" s="4"/>
       <c r="BH17" s="4"/>
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
-      <c r="BO17" s="3"/>
+      <c r="BK17" s="4"/>
       <c r="BP17" s="3"/>
       <c r="BQ17" s="3"/>
-      <c r="BR17" s="3"/>
-      <c r="BS17" s="3"/>
-    </row>
-    <row r="18" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AG18" s="4"/>
       <c r="AJ18" s="4"/>
@@ -1896,26 +1920,25 @@
       <c r="AS18" s="4"/>
       <c r="AT18" s="4"/>
       <c r="AU18" s="4"/>
+      <c r="AV18" s="4"/>
+      <c r="AW18" s="4"/>
       <c r="AX18" s="4"/>
       <c r="AY18" s="4"/>
       <c r="AZ18" s="4"/>
-      <c r="BA18" s="4"/>
-      <c r="BB18" s="4"/>
-      <c r="BE18" s="4"/>
       <c r="BF18" s="4"/>
       <c r="BG18" s="4"/>
       <c r="BH18" s="4"/>
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
+      <c r="BK18" s="4"/>
+      <c r="BR18" s="3"/>
+      <c r="BS18" s="3"/>
       <c r="BT18" s="3"/>
       <c r="BU18" s="3"/>
-      <c r="BV18" s="3"/>
-      <c r="BW18" s="3"/>
-      <c r="BX18" s="3"/>
-    </row>
-    <row r="19" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AG19" s="4"/>
       <c r="AJ19" s="4"/>
@@ -1928,23 +1951,21 @@
       <c r="AS19" s="4"/>
       <c r="AT19" s="4"/>
       <c r="AU19" s="4"/>
+      <c r="AV19" s="4"/>
+      <c r="AW19" s="4"/>
       <c r="AX19" s="4"/>
       <c r="AY19" s="4"/>
       <c r="AZ19" s="4"/>
       <c r="BA19" s="4"/>
       <c r="BB19" s="4"/>
+      <c r="BC19" s="4"/>
+      <c r="BD19" s="4"/>
       <c r="BE19" s="4"/>
       <c r="BF19" s="4"/>
-      <c r="BG19" s="4"/>
-      <c r="BH19" s="4"/>
-      <c r="BI19" s="4"/>
-      <c r="BJ19" s="4"/>
-      <c r="BX19" s="4"/>
-      <c r="BY19" s="4"/>
-      <c r="BZ19" s="4"/>
-      <c r="CA19" s="4"/>
-      <c r="CB19" s="4"/>
-      <c r="CC19" s="4"/>
+      <c r="BZ19" s="3"/>
+      <c r="CA19" s="3"/>
+      <c r="CB19" s="3"/>
+      <c r="CC19" s="3"/>
       <c r="CD19" s="3"/>
       <c r="CE19" s="3"/>
       <c r="CF19" s="3"/>
@@ -1956,33 +1977,29 @@
       <c r="CL19" s="3"/>
       <c r="CM19" s="3"/>
       <c r="CN19" s="3"/>
-      <c r="CO19" s="3"/>
-      <c r="CP19" s="3"/>
-      <c r="CQ19" s="3"/>
-      <c r="CR19" s="3"/>
-      <c r="CS19" s="4"/>
-      <c r="CT19" s="4"/>
-    </row>
-    <row r="20" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CO19" s="4"/>
+      <c r="CP19" s="4"/>
+    </row>
+    <row r="20" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="CU20" s="3"/>
-      <c r="CV20" s="3"/>
-      <c r="CW20" s="3"/>
-    </row>
-    <row r="21" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:101" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>21</v>
+      </c>
+      <c r="CQ20" s="3"/>
+      <c r="CR20" s="3"/>
+      <c r="CS20" s="3"/>
+    </row>
+    <row r="21" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -1990,21 +2007,1019 @@
     <mergeCell ref="AC1:AG1"/>
     <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="AQ1:AU1"/>
-    <mergeCell ref="AX1:BB1"/>
+    <mergeCell ref="AV1:AZ1"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="CI1:CM1"/>
-    <mergeCell ref="CN1:CR1"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="BE1:BI1"/>
-    <mergeCell ref="BJ1:BN1"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BT1:BX1"/>
-    <mergeCell ref="BY1:CC1"/>
-    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CO1:CS1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BO1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CD1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3CD27E-A115-4399-987E-8115A89C15E2}">
+  <dimension ref="A1:CT33"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.6328125" style="2" customWidth="1"/>
+    <col min="2" max="20" width="2.81640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="2.81640625" style="7" hidden="1" customWidth="1"/>
+    <col min="22" max="44" width="2.81640625" hidden="1" customWidth="1"/>
+    <col min="45" max="47" width="2.7265625" hidden="1" customWidth="1"/>
+    <col min="48" max="97" width="2.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:98" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="22">
+        <v>43276</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22">
+        <v>43283</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22">
+        <v>43290</v>
+      </c>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22">
+        <v>43297</v>
+      </c>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23">
+        <v>43304</v>
+      </c>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="24">
+        <v>43311</v>
+      </c>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="21"/>
+      <c r="AJ1" s="24">
+        <v>43318</v>
+      </c>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="20"/>
+      <c r="AP1" s="21"/>
+      <c r="AQ1" s="23">
+        <v>43325</v>
+      </c>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="24">
+        <v>43332</v>
+      </c>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="22">
+        <v>43339</v>
+      </c>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22">
+        <v>43346</v>
+      </c>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22">
+        <v>43353</v>
+      </c>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22">
+        <v>43360</v>
+      </c>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22">
+        <v>43367</v>
+      </c>
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22">
+        <v>43374</v>
+      </c>
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
+      <c r="CC1" s="22"/>
+      <c r="CD1" s="22"/>
+      <c r="CE1" s="22">
+        <v>43381</v>
+      </c>
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22">
+        <v>43388</v>
+      </c>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="23"/>
+      <c r="CO1" s="22">
+        <v>43395</v>
+      </c>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="23"/>
+    </row>
+    <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12"/>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BG2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BV2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BY2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BZ2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CB2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="CC2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CD2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="CF2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CG2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CI2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="CJ2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="CK2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CL2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="CM2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CN2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CO2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="CP2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CQ2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="CR2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="CS2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CT2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="CT3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="I4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+    </row>
+    <row r="6" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="8"/>
+      <c r="W6" s="4"/>
+    </row>
+    <row r="7" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="4"/>
+    </row>
+    <row r="8" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AO8" s="4"/>
+      <c r="AP8" s="4"/>
+    </row>
+    <row r="9" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="4"/>
+      <c r="AP9" s="4"/>
+    </row>
+    <row r="10" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+    </row>
+    <row r="11" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AO11" s="4"/>
+      <c r="AS11" s="3"/>
+    </row>
+    <row r="12" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="4"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="4"/>
+      <c r="AT12" s="3"/>
+      <c r="AU12" s="3"/>
+      <c r="AV12" s="3"/>
+      <c r="AW12" s="3"/>
+      <c r="AX12" s="3"/>
+      <c r="AY12" s="3"/>
+      <c r="AZ12" s="3"/>
+    </row>
+    <row r="13" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="BA13" s="3"/>
+      <c r="BB13" s="3"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+    </row>
+    <row r="14" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
+      <c r="BJ14" s="3"/>
+    </row>
+    <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG15" s="4"/>
+      <c r="AJ15" s="4"/>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="4"/>
+      <c r="AN15" s="4"/>
+      <c r="AQ15" s="4"/>
+      <c r="AR15" s="4"/>
+      <c r="AS15" s="4"/>
+      <c r="AT15" s="4"/>
+      <c r="AU15" s="4"/>
+      <c r="AV15" s="4"/>
+      <c r="AW15" s="4"/>
+      <c r="AX15" s="4"/>
+      <c r="AY15" s="4"/>
+      <c r="AZ15" s="4"/>
+      <c r="BF15" s="4"/>
+      <c r="BG15" s="4"/>
+      <c r="BH15" s="4"/>
+      <c r="BI15" s="4"/>
+      <c r="BJ15" s="4"/>
+      <c r="BK15" s="3"/>
+      <c r="BL15" s="3"/>
+      <c r="BM15" s="3"/>
+      <c r="BN15" s="3"/>
+      <c r="BO15" s="3"/>
+    </row>
+    <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG16" s="4"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="4"/>
+      <c r="AL16" s="4"/>
+      <c r="AM16" s="4"/>
+      <c r="AN16" s="4"/>
+      <c r="AQ16" s="4"/>
+      <c r="AR16" s="4"/>
+      <c r="AS16" s="4"/>
+      <c r="AT16" s="4"/>
+      <c r="AU16" s="4"/>
+      <c r="AV16" s="4"/>
+      <c r="AW16" s="4"/>
+      <c r="AX16" s="4"/>
+      <c r="AY16" s="4"/>
+      <c r="AZ16" s="4"/>
+      <c r="BF16" s="4"/>
+      <c r="BG16" s="4"/>
+      <c r="BH16" s="4"/>
+      <c r="BI16" s="4"/>
+      <c r="BJ16" s="4"/>
+      <c r="BK16" s="4"/>
+      <c r="BP16" s="3"/>
+      <c r="BQ16" s="3"/>
+      <c r="BR16" s="3"/>
+      <c r="BS16" s="3"/>
+      <c r="BT16" s="3"/>
+    </row>
+    <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="4"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="4"/>
+      <c r="AN17" s="4"/>
+      <c r="AQ17" s="4"/>
+      <c r="AR17" s="4"/>
+      <c r="AS17" s="4"/>
+      <c r="AT17" s="4"/>
+      <c r="AU17" s="4"/>
+      <c r="AV17" s="4"/>
+      <c r="AW17" s="4"/>
+      <c r="AX17" s="4"/>
+      <c r="AY17" s="4"/>
+      <c r="AZ17" s="4"/>
+      <c r="BF17" s="4"/>
+      <c r="BG17" s="4"/>
+      <c r="BH17" s="4"/>
+      <c r="BI17" s="4"/>
+      <c r="BJ17" s="4"/>
+      <c r="BK17" s="4"/>
+      <c r="BU17" s="3"/>
+      <c r="BV17" s="3"/>
+      <c r="BW17" s="3"/>
+      <c r="BX17" s="3"/>
+      <c r="BY17" s="3"/>
+    </row>
+    <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="4"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+      <c r="AN18" s="4"/>
+      <c r="AQ18" s="4"/>
+      <c r="AR18" s="4"/>
+      <c r="AS18" s="4"/>
+      <c r="AT18" s="4"/>
+      <c r="AU18" s="4"/>
+      <c r="AV18" s="4"/>
+      <c r="AW18" s="4"/>
+      <c r="AX18" s="4"/>
+      <c r="AY18" s="4"/>
+      <c r="AZ18" s="4"/>
+      <c r="BA18" s="4"/>
+      <c r="BB18" s="4"/>
+      <c r="BC18" s="4"/>
+      <c r="BD18" s="4"/>
+      <c r="BE18" s="4"/>
+      <c r="BF18" s="4"/>
+      <c r="BT18" s="4"/>
+      <c r="BU18" s="4"/>
+      <c r="BV18" s="4"/>
+      <c r="BW18" s="4"/>
+      <c r="BX18" s="4"/>
+      <c r="BY18" s="4"/>
+      <c r="BZ18" s="3"/>
+      <c r="CA18" s="3"/>
+      <c r="CB18" s="3"/>
+      <c r="CC18" s="3"/>
+      <c r="CD18" s="3"/>
+      <c r="CE18" s="3"/>
+      <c r="CF18" s="3"/>
+      <c r="CG18" s="3"/>
+      <c r="CH18" s="3"/>
+      <c r="CI18" s="3"/>
+      <c r="CJ18" s="3"/>
+      <c r="CK18" s="3"/>
+      <c r="CL18" s="3"/>
+      <c r="CM18" s="3"/>
+      <c r="CN18" s="3"/>
+      <c r="CO18" s="4"/>
+      <c r="CP18" s="4"/>
+    </row>
+    <row r="19" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="CQ19" s="3"/>
+      <c r="CR19" s="3"/>
+      <c r="CS19" s="3"/>
+    </row>
+    <row r="20" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="CO1:CS1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AQ1:AU1"/>
+    <mergeCell ref="AV1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BO1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CD1"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add some work on thesis doc
</commit_message>
<xml_diff>
--- a/Thesis Project - Gantt Chart.xlsx
+++ b/Thesis Project - Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\EEE4022S Thesis Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8C057-16FD-4F46-8E32-519A43A4D032}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05D5EF7-BBDC-4AFF-A42A-BF606709F713}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8860" xr2:uid="{A2B2673A-199A-4790-994A-444B0E0296E2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="32">
   <si>
     <t>T</t>
   </si>
@@ -517,12 +517,67 @@
       <t xml:space="preserve"> compare options, order</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rpi to gimbal comms: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>create and test serialAPI</t>
+    </r>
+  </si>
+  <si>
+    <t>Misc to do</t>
+  </si>
+  <si>
+    <t>power Rpi from gimbal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do tests:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in lab, put on quad, animals, etc</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +596,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -613,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,6 +730,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -997,8 +1063,8 @@
   <dimension ref="A1:CT34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BG14" sqref="BG14"/>
+      <pane xSplit="1" topLeftCell="BK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BO16" sqref="BO16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,146 +1073,146 @@
     <col min="2" max="20" width="2.81640625" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="2.81640625" style="7" hidden="1" customWidth="1"/>
     <col min="22" max="44" width="2.81640625" hidden="1" customWidth="1"/>
-    <col min="45" max="57" width="2.7265625" hidden="1" customWidth="1"/>
-    <col min="58" max="97" width="2.7265625" customWidth="1"/>
+    <col min="45" max="62" width="2.7265625" hidden="1" customWidth="1"/>
+    <col min="63" max="97" width="2.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="23">
         <v>43276</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23">
         <v>43283</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23">
         <v>43290</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22">
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23">
         <v>43297</v>
       </c>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23">
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24">
         <v>43304</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
       <c r="AA1" s="15"/>
       <c r="AB1" s="14"/>
-      <c r="AC1" s="24">
+      <c r="AC1" s="25">
         <v>43311</v>
       </c>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
       <c r="AH1" s="15"/>
       <c r="AI1" s="16"/>
-      <c r="AJ1" s="24">
+      <c r="AJ1" s="25">
         <v>43318</v>
       </c>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
       <c r="AO1" s="17"/>
       <c r="AP1" s="16"/>
-      <c r="AQ1" s="23">
+      <c r="AQ1" s="24">
         <v>43325</v>
       </c>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="24">
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="25">
         <v>43332</v>
       </c>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="22">
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="23">
         <v>43339</v>
       </c>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22">
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23">
         <v>43346</v>
       </c>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22">
+      <c r="BG1" s="23"/>
+      <c r="BH1" s="23"/>
+      <c r="BI1" s="23"/>
+      <c r="BJ1" s="23"/>
+      <c r="BK1" s="23">
         <v>43353</v>
       </c>
-      <c r="BL1" s="22"/>
-      <c r="BM1" s="22"/>
-      <c r="BN1" s="22"/>
-      <c r="BO1" s="22"/>
-      <c r="BP1" s="22">
+      <c r="BL1" s="23"/>
+      <c r="BM1" s="23"/>
+      <c r="BN1" s="23"/>
+      <c r="BO1" s="23"/>
+      <c r="BP1" s="23">
         <v>43360</v>
       </c>
-      <c r="BQ1" s="22"/>
-      <c r="BR1" s="22"/>
-      <c r="BS1" s="22"/>
-      <c r="BT1" s="22"/>
-      <c r="BU1" s="22">
+      <c r="BQ1" s="23"/>
+      <c r="BR1" s="23"/>
+      <c r="BS1" s="23"/>
+      <c r="BT1" s="23"/>
+      <c r="BU1" s="23">
         <v>43367</v>
       </c>
-      <c r="BV1" s="22"/>
-      <c r="BW1" s="22"/>
-      <c r="BX1" s="22"/>
-      <c r="BY1" s="22"/>
-      <c r="BZ1" s="22">
+      <c r="BV1" s="23"/>
+      <c r="BW1" s="23"/>
+      <c r="BX1" s="23"/>
+      <c r="BY1" s="23"/>
+      <c r="BZ1" s="23">
         <v>43374</v>
       </c>
-      <c r="CA1" s="22"/>
-      <c r="CB1" s="22"/>
-      <c r="CC1" s="22"/>
-      <c r="CD1" s="22"/>
-      <c r="CE1" s="22">
+      <c r="CA1" s="23"/>
+      <c r="CB1" s="23"/>
+      <c r="CC1" s="23"/>
+      <c r="CD1" s="23"/>
+      <c r="CE1" s="23">
         <v>43381</v>
       </c>
-      <c r="CF1" s="22"/>
-      <c r="CG1" s="22"/>
-      <c r="CH1" s="22"/>
-      <c r="CI1" s="22"/>
-      <c r="CJ1" s="22">
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="23"/>
+      <c r="CI1" s="23"/>
+      <c r="CJ1" s="23">
         <v>43388</v>
       </c>
-      <c r="CK1" s="22"/>
-      <c r="CL1" s="22"/>
-      <c r="CM1" s="22"/>
-      <c r="CN1" s="23"/>
-      <c r="CO1" s="22">
+      <c r="CK1" s="23"/>
+      <c r="CL1" s="23"/>
+      <c r="CM1" s="23"/>
+      <c r="CN1" s="24"/>
+      <c r="CO1" s="23">
         <v>43395</v>
       </c>
-      <c r="CP1" s="22"/>
-      <c r="CQ1" s="22"/>
-      <c r="CR1" s="22"/>
-      <c r="CS1" s="23"/>
+      <c r="CP1" s="23"/>
+      <c r="CQ1" s="23"/>
+      <c r="CR1" s="23"/>
+      <c r="CS1" s="24"/>
     </row>
     <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
@@ -1741,7 +1807,7 @@
       <c r="AY12" s="3"/>
       <c r="AZ12" s="3"/>
     </row>
-    <row r="13" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1788,9 +1854,6 @@
       <c r="BF13" s="3"/>
       <c r="BG13" s="3"/>
       <c r="BH13" s="3"/>
-      <c r="BI13" s="3"/>
-      <c r="BJ13" s="3"/>
-      <c r="BK13" s="3"/>
     </row>
     <row r="14" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
@@ -1816,11 +1879,16 @@
       <c r="X14" s="4"/>
       <c r="BH14" s="3"/>
       <c r="BI14" s="3"/>
-      <c r="BJ14" s="3"/>
+      <c r="BL14" s="3"/>
+      <c r="BM14" s="3"/>
+      <c r="BN14" s="3"/>
+      <c r="BO14" s="3"/>
+      <c r="BP14" s="3"/>
+      <c r="BQ14" s="3"/>
     </row>
     <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
+      <c r="A15" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1840,10 +1908,12 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
+      <c r="BH15" s="3"/>
+      <c r="BI15" s="3"/>
+      <c r="BJ15" s="3"/>
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
-      <c r="BN15" s="3"/>
     </row>
     <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
@@ -1873,8 +1943,13 @@
       <c r="BK16" s="4"/>
       <c r="BL16" s="4"/>
       <c r="BM16" s="4"/>
-      <c r="BN16" s="3"/>
-      <c r="BO16" s="3"/>
+      <c r="BN16" s="4"/>
+      <c r="BO16" s="4"/>
+      <c r="BP16" s="3"/>
+      <c r="BQ16" s="3"/>
+      <c r="BR16" s="3"/>
+      <c r="BS16" s="3"/>
+      <c r="BT16" s="3"/>
     </row>
     <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
@@ -1902,12 +1977,12 @@
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
       <c r="BK17" s="4"/>
-      <c r="BP17" s="3"/>
-      <c r="BQ17" s="3"/>
+      <c r="BU17" s="3"/>
+      <c r="BV17" s="3"/>
     </row>
     <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="AG18" s="4"/>
       <c r="AJ18" s="4"/>
@@ -1931,10 +2006,15 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
-      <c r="BR18" s="3"/>
-      <c r="BS18" s="3"/>
-      <c r="BT18" s="3"/>
-      <c r="BU18" s="3"/>
+      <c r="BV18" s="3"/>
+      <c r="BW18" s="3"/>
+      <c r="BX18" s="3"/>
+      <c r="BY18" s="3"/>
+      <c r="BZ18" s="3"/>
+      <c r="CA18" s="3"/>
+      <c r="CB18" s="3"/>
+      <c r="CC18" s="3"/>
+      <c r="CD18" s="3"/>
     </row>
     <row r="19" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
@@ -1990,7 +2070,14 @@
     </row>
     <row r="21" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BK23" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="24" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2033,8 +2120,8 @@
   <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BC20" sqref="BC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2051,138 +2138,138 @@
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="23">
         <v>43276</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23">
         <v>43283</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23">
         <v>43290</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22">
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23">
         <v>43297</v>
       </c>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23">
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24">
         <v>43304</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
       <c r="AA1" s="20"/>
       <c r="AB1" s="21"/>
-      <c r="AC1" s="24">
+      <c r="AC1" s="25">
         <v>43311</v>
       </c>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
       <c r="AH1" s="20"/>
       <c r="AI1" s="21"/>
-      <c r="AJ1" s="24">
+      <c r="AJ1" s="25">
         <v>43318</v>
       </c>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="21"/>
-      <c r="AQ1" s="23">
+      <c r="AQ1" s="24">
         <v>43325</v>
       </c>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="24">
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="25">
         <v>43332</v>
       </c>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="22">
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="23">
         <v>43339</v>
       </c>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22">
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23">
         <v>43346</v>
       </c>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22">
+      <c r="BG1" s="23"/>
+      <c r="BH1" s="23"/>
+      <c r="BI1" s="23"/>
+      <c r="BJ1" s="23"/>
+      <c r="BK1" s="23">
         <v>43353</v>
       </c>
-      <c r="BL1" s="22"/>
-      <c r="BM1" s="22"/>
-      <c r="BN1" s="22"/>
-      <c r="BO1" s="22"/>
-      <c r="BP1" s="22">
+      <c r="BL1" s="23"/>
+      <c r="BM1" s="23"/>
+      <c r="BN1" s="23"/>
+      <c r="BO1" s="23"/>
+      <c r="BP1" s="23">
         <v>43360</v>
       </c>
-      <c r="BQ1" s="22"/>
-      <c r="BR1" s="22"/>
-      <c r="BS1" s="22"/>
-      <c r="BT1" s="22"/>
-      <c r="BU1" s="22">
+      <c r="BQ1" s="23"/>
+      <c r="BR1" s="23"/>
+      <c r="BS1" s="23"/>
+      <c r="BT1" s="23"/>
+      <c r="BU1" s="23">
         <v>43367</v>
       </c>
-      <c r="BV1" s="22"/>
-      <c r="BW1" s="22"/>
-      <c r="BX1" s="22"/>
-      <c r="BY1" s="22"/>
-      <c r="BZ1" s="22">
+      <c r="BV1" s="23"/>
+      <c r="BW1" s="23"/>
+      <c r="BX1" s="23"/>
+      <c r="BY1" s="23"/>
+      <c r="BZ1" s="23">
         <v>43374</v>
       </c>
-      <c r="CA1" s="22"/>
-      <c r="CB1" s="22"/>
-      <c r="CC1" s="22"/>
-      <c r="CD1" s="22"/>
-      <c r="CE1" s="22">
+      <c r="CA1" s="23"/>
+      <c r="CB1" s="23"/>
+      <c r="CC1" s="23"/>
+      <c r="CD1" s="23"/>
+      <c r="CE1" s="23">
         <v>43381</v>
       </c>
-      <c r="CF1" s="22"/>
-      <c r="CG1" s="22"/>
-      <c r="CH1" s="22"/>
-      <c r="CI1" s="22"/>
-      <c r="CJ1" s="22">
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="23"/>
+      <c r="CI1" s="23"/>
+      <c r="CJ1" s="23">
         <v>43388</v>
       </c>
-      <c r="CK1" s="22"/>
-      <c r="CL1" s="22"/>
-      <c r="CM1" s="22"/>
-      <c r="CN1" s="23"/>
-      <c r="CO1" s="22">
+      <c r="CK1" s="23"/>
+      <c r="CL1" s="23"/>
+      <c r="CM1" s="23"/>
+      <c r="CN1" s="24"/>
+      <c r="CO1" s="23">
         <v>43395</v>
       </c>
-      <c r="CP1" s="22"/>
-      <c r="CQ1" s="22"/>
-      <c r="CR1" s="22"/>
-      <c r="CS1" s="23"/>
+      <c r="CP1" s="23"/>
+      <c r="CQ1" s="23"/>
+      <c r="CR1" s="23"/>
+      <c r="CS1" s="24"/>
     </row>
     <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>

</xml_diff>

<commit_message>
Update Gantt chart and sources.txt
</commit_message>
<xml_diff>
--- a/Thesis Project - Gantt Chart.xlsx
+++ b/Thesis Project - Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\EEE4022S Thesis Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05D5EF7-BBDC-4AFF-A42A-BF606709F713}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3AC497-FFA7-49C8-B9B1-FB71133161A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8860" xr2:uid="{A2B2673A-199A-4790-994A-444B0E0296E2}"/>
   </bookViews>
@@ -1064,7 +1064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BO16" sqref="BO16"/>
+      <selection pane="topRight" activeCell="BV20" sqref="BV20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,8 +1073,8 @@
     <col min="2" max="20" width="2.81640625" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="2.81640625" style="7" hidden="1" customWidth="1"/>
     <col min="22" max="44" width="2.81640625" hidden="1" customWidth="1"/>
-    <col min="45" max="62" width="2.7265625" hidden="1" customWidth="1"/>
-    <col min="63" max="97" width="2.7265625" customWidth="1"/>
+    <col min="45" max="67" width="2.7265625" hidden="1" customWidth="1"/>
+    <col min="68" max="97" width="2.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:98" x14ac:dyDescent="0.35">
@@ -1883,8 +1883,8 @@
       <c r="BM14" s="3"/>
       <c r="BN14" s="3"/>
       <c r="BO14" s="3"/>
-      <c r="BP14" s="3"/>
       <c r="BQ14" s="3"/>
+      <c r="BR14" s="3"/>
     </row>
     <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
@@ -1914,6 +1914,8 @@
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
+      <c r="BQ15" s="3"/>
+      <c r="BR15" s="3"/>
     </row>
     <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
@@ -1945,11 +1947,12 @@
       <c r="BM16" s="4"/>
       <c r="BN16" s="4"/>
       <c r="BO16" s="4"/>
-      <c r="BP16" s="3"/>
-      <c r="BQ16" s="3"/>
       <c r="BR16" s="3"/>
       <c r="BS16" s="3"/>
       <c r="BT16" s="3"/>
+      <c r="BU16" s="3"/>
+      <c r="BV16" s="3"/>
+      <c r="BW16" s="3"/>
     </row>
     <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
@@ -1977,8 +1980,8 @@
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
       <c r="BK17" s="4"/>
-      <c r="BU17" s="3"/>
-      <c r="BV17" s="3"/>
+      <c r="BZ17" s="3"/>
+      <c r="CA17" s="3"/>
     </row>
     <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
@@ -2006,7 +2009,6 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
-      <c r="BV18" s="3"/>
       <c r="BW18" s="3"/>
       <c r="BX18" s="3"/>
       <c r="BY18" s="3"/>
@@ -2042,6 +2044,12 @@
       <c r="BD19" s="4"/>
       <c r="BE19" s="4"/>
       <c r="BF19" s="4"/>
+      <c r="BT19" s="3"/>
+      <c r="BU19" s="3"/>
+      <c r="BV19" s="3"/>
+      <c r="BW19" s="3"/>
+      <c r="BX19" s="3"/>
+      <c r="BY19" s="3"/>
       <c r="BZ19" s="3"/>
       <c r="CA19" s="3"/>
       <c r="CB19" s="3"/>

</xml_diff>

<commit_message>
Work on paper + EKF
</commit_message>
<xml_diff>
--- a/Thesis Project - Gantt Chart.xlsx
+++ b/Thesis Project - Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\EEE4022S Thesis Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3AC497-FFA7-49C8-B9B1-FB71133161A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6047A07F-471B-45AF-9E68-8F5DDE9A76B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8860" xr2:uid="{A2B2673A-199A-4790-994A-444B0E0296E2}"/>
   </bookViews>
@@ -734,16 +734,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1064,7 +1064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BV20" sqref="BV20"/>
+      <selection pane="topRight" activeCell="BX18" sqref="BX18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,137 +1081,137 @@
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="23">
+      <c r="B1" s="26">
         <v>43276</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26">
         <v>43283</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26">
         <v>43290</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23">
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26">
         <v>43297</v>
       </c>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
       <c r="U1" s="24"/>
       <c r="V1" s="24">
         <v>43304</v>
       </c>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
       <c r="AA1" s="15"/>
       <c r="AB1" s="14"/>
-      <c r="AC1" s="25">
+      <c r="AC1" s="23">
         <v>43311</v>
       </c>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
       <c r="AH1" s="15"/>
       <c r="AI1" s="16"/>
-      <c r="AJ1" s="25">
+      <c r="AJ1" s="23">
         <v>43318</v>
       </c>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
       <c r="AO1" s="17"/>
       <c r="AP1" s="16"/>
       <c r="AQ1" s="24">
         <v>43325</v>
       </c>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="25"/>
-      <c r="AU1" s="26"/>
-      <c r="AV1" s="25">
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="23">
         <v>43332</v>
       </c>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="25"/>
-      <c r="AZ1" s="25"/>
-      <c r="BA1" s="23">
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="23"/>
+      <c r="AZ1" s="23"/>
+      <c r="BA1" s="26">
         <v>43339</v>
       </c>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23">
+      <c r="BB1" s="26"/>
+      <c r="BC1" s="26"/>
+      <c r="BD1" s="26"/>
+      <c r="BE1" s="26"/>
+      <c r="BF1" s="26">
         <v>43346</v>
       </c>
-      <c r="BG1" s="23"/>
-      <c r="BH1" s="23"/>
-      <c r="BI1" s="23"/>
-      <c r="BJ1" s="23"/>
-      <c r="BK1" s="23">
+      <c r="BG1" s="26"/>
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="26"/>
+      <c r="BJ1" s="26"/>
+      <c r="BK1" s="26">
         <v>43353</v>
       </c>
-      <c r="BL1" s="23"/>
-      <c r="BM1" s="23"/>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23">
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="26"/>
+      <c r="BO1" s="26"/>
+      <c r="BP1" s="26">
         <v>43360</v>
       </c>
-      <c r="BQ1" s="23"/>
-      <c r="BR1" s="23"/>
-      <c r="BS1" s="23"/>
-      <c r="BT1" s="23"/>
-      <c r="BU1" s="23">
+      <c r="BQ1" s="26"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="26"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="26">
         <v>43367</v>
       </c>
-      <c r="BV1" s="23"/>
-      <c r="BW1" s="23"/>
-      <c r="BX1" s="23"/>
-      <c r="BY1" s="23"/>
-      <c r="BZ1" s="23">
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26">
         <v>43374</v>
       </c>
-      <c r="CA1" s="23"/>
-      <c r="CB1" s="23"/>
-      <c r="CC1" s="23"/>
-      <c r="CD1" s="23"/>
-      <c r="CE1" s="23">
+      <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
+      <c r="CC1" s="26"/>
+      <c r="CD1" s="26"/>
+      <c r="CE1" s="26">
         <v>43381</v>
       </c>
-      <c r="CF1" s="23"/>
-      <c r="CG1" s="23"/>
-      <c r="CH1" s="23"/>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23">
+      <c r="CF1" s="26"/>
+      <c r="CG1" s="26"/>
+      <c r="CH1" s="26"/>
+      <c r="CI1" s="26"/>
+      <c r="CJ1" s="26">
         <v>43388</v>
       </c>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CM1" s="23"/>
+      <c r="CK1" s="26"/>
+      <c r="CL1" s="26"/>
+      <c r="CM1" s="26"/>
       <c r="CN1" s="24"/>
-      <c r="CO1" s="23">
+      <c r="CO1" s="26">
         <v>43395</v>
       </c>
-      <c r="CP1" s="23"/>
-      <c r="CQ1" s="23"/>
-      <c r="CR1" s="23"/>
+      <c r="CP1" s="26"/>
+      <c r="CQ1" s="26"/>
+      <c r="CR1" s="26"/>
       <c r="CS1" s="24"/>
     </row>
     <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1950,9 +1950,8 @@
       <c r="BR16" s="3"/>
       <c r="BS16" s="3"/>
       <c r="BT16" s="3"/>
-      <c r="BU16" s="3"/>
-      <c r="BV16" s="3"/>
       <c r="BW16" s="3"/>
+      <c r="BX16" s="3"/>
     </row>
     <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
@@ -2009,7 +2008,6 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
-      <c r="BW18" s="3"/>
       <c r="BX18" s="3"/>
       <c r="BY18" s="3"/>
       <c r="BZ18" s="3"/>
@@ -2099,6 +2097,15 @@
     <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CO1:CS1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BO1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CD1"/>
     <mergeCell ref="AC1:AG1"/>
     <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="AQ1:AU1"/>
@@ -2108,15 +2115,6 @@
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="CE1:CI1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CO1:CS1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BO1"/>
-    <mergeCell ref="BP1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
-    <mergeCell ref="BZ1:CD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2146,137 +2144,137 @@
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="23">
+      <c r="B1" s="26">
         <v>43276</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26">
         <v>43283</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26">
         <v>43290</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23">
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26">
         <v>43297</v>
       </c>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
       <c r="U1" s="24"/>
       <c r="V1" s="24">
         <v>43304</v>
       </c>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
       <c r="AA1" s="20"/>
       <c r="AB1" s="21"/>
-      <c r="AC1" s="25">
+      <c r="AC1" s="23">
         <v>43311</v>
       </c>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
       <c r="AH1" s="20"/>
       <c r="AI1" s="21"/>
-      <c r="AJ1" s="25">
+      <c r="AJ1" s="23">
         <v>43318</v>
       </c>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="21"/>
       <c r="AQ1" s="24">
         <v>43325</v>
       </c>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="25"/>
-      <c r="AU1" s="26"/>
-      <c r="AV1" s="25">
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="23">
         <v>43332</v>
       </c>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="25"/>
-      <c r="AZ1" s="25"/>
-      <c r="BA1" s="23">
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="23"/>
+      <c r="AZ1" s="23"/>
+      <c r="BA1" s="26">
         <v>43339</v>
       </c>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23">
+      <c r="BB1" s="26"/>
+      <c r="BC1" s="26"/>
+      <c r="BD1" s="26"/>
+      <c r="BE1" s="26"/>
+      <c r="BF1" s="26">
         <v>43346</v>
       </c>
-      <c r="BG1" s="23"/>
-      <c r="BH1" s="23"/>
-      <c r="BI1" s="23"/>
-      <c r="BJ1" s="23"/>
-      <c r="BK1" s="23">
+      <c r="BG1" s="26"/>
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="26"/>
+      <c r="BJ1" s="26"/>
+      <c r="BK1" s="26">
         <v>43353</v>
       </c>
-      <c r="BL1" s="23"/>
-      <c r="BM1" s="23"/>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23">
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="26"/>
+      <c r="BO1" s="26"/>
+      <c r="BP1" s="26">
         <v>43360</v>
       </c>
-      <c r="BQ1" s="23"/>
-      <c r="BR1" s="23"/>
-      <c r="BS1" s="23"/>
-      <c r="BT1" s="23"/>
-      <c r="BU1" s="23">
+      <c r="BQ1" s="26"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="26"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="26">
         <v>43367</v>
       </c>
-      <c r="BV1" s="23"/>
-      <c r="BW1" s="23"/>
-      <c r="BX1" s="23"/>
-      <c r="BY1" s="23"/>
-      <c r="BZ1" s="23">
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26">
         <v>43374</v>
       </c>
-      <c r="CA1" s="23"/>
-      <c r="CB1" s="23"/>
-      <c r="CC1" s="23"/>
-      <c r="CD1" s="23"/>
-      <c r="CE1" s="23">
+      <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
+      <c r="CC1" s="26"/>
+      <c r="CD1" s="26"/>
+      <c r="CE1" s="26">
         <v>43381</v>
       </c>
-      <c r="CF1" s="23"/>
-      <c r="CG1" s="23"/>
-      <c r="CH1" s="23"/>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23">
+      <c r="CF1" s="26"/>
+      <c r="CG1" s="26"/>
+      <c r="CH1" s="26"/>
+      <c r="CI1" s="26"/>
+      <c r="CJ1" s="26">
         <v>43388</v>
       </c>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CM1" s="23"/>
+      <c r="CK1" s="26"/>
+      <c r="CL1" s="26"/>
+      <c r="CM1" s="26"/>
       <c r="CN1" s="24"/>
-      <c r="CO1" s="23">
+      <c r="CO1" s="26">
         <v>43395</v>
       </c>
-      <c r="CP1" s="23"/>
-      <c r="CQ1" s="23"/>
-      <c r="CR1" s="23"/>
+      <c r="CP1" s="26"/>
+      <c r="CQ1" s="26"/>
+      <c r="CR1" s="26"/>
       <c r="CS1" s="24"/>
     </row>
     <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -3097,6 +3095,12 @@
     <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
     <mergeCell ref="CO1:CS1"/>
     <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="AQ1:AU1"/>
@@ -3109,12 +3113,6 @@
     <mergeCell ref="BZ1:CD1"/>
     <mergeCell ref="CE1:CI1"/>
     <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Expanded Gantt chart to full view. It wasn't used much in the last few weeks of the project
</commit_message>
<xml_diff>
--- a/Thesis Project - Gantt Chart.xlsx
+++ b/Thesis Project - Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\EEE4022S Thesis Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6047A07F-471B-45AF-9E68-8F5DDE9A76B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1357F2AB-36FE-4DC3-83F7-72BEFC3641CC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8860" xr2:uid="{A2B2673A-199A-4790-994A-444B0E0296E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8856" xr2:uid="{A2B2673A-199A-4790-994A-444B0E0296E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -734,16 +734,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1063,158 +1063,156 @@
   <dimension ref="A1:CT34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BX18" sqref="BX18"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" style="2" customWidth="1"/>
-    <col min="2" max="20" width="2.81640625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="2.81640625" style="7" hidden="1" customWidth="1"/>
-    <col min="22" max="44" width="2.81640625" hidden="1" customWidth="1"/>
-    <col min="45" max="67" width="2.7265625" hidden="1" customWidth="1"/>
-    <col min="68" max="97" width="2.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="20" width="2.77734375" customWidth="1"/>
+    <col min="21" max="21" width="2.77734375" style="7" customWidth="1"/>
+    <col min="22" max="97" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="26">
+      <c r="B1" s="23">
         <v>43276</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23">
         <v>43283</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23">
         <v>43290</v>
       </c>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26">
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23">
         <v>43297</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
       <c r="U1" s="24"/>
       <c r="V1" s="24">
         <v>43304</v>
       </c>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
       <c r="AA1" s="15"/>
       <c r="AB1" s="14"/>
-      <c r="AC1" s="23">
+      <c r="AC1" s="25">
         <v>43311</v>
       </c>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
       <c r="AH1" s="15"/>
       <c r="AI1" s="16"/>
-      <c r="AJ1" s="23">
+      <c r="AJ1" s="25">
         <v>43318</v>
       </c>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
       <c r="AO1" s="17"/>
       <c r="AP1" s="16"/>
       <c r="AQ1" s="24">
         <v>43325</v>
       </c>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="23">
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="25">
         <v>43332</v>
       </c>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="26">
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="23">
         <v>43339</v>
       </c>
-      <c r="BB1" s="26"/>
-      <c r="BC1" s="26"/>
-      <c r="BD1" s="26"/>
-      <c r="BE1" s="26"/>
-      <c r="BF1" s="26">
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23">
         <v>43346</v>
       </c>
-      <c r="BG1" s="26"/>
-      <c r="BH1" s="26"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="26"/>
-      <c r="BK1" s="26">
+      <c r="BG1" s="23"/>
+      <c r="BH1" s="23"/>
+      <c r="BI1" s="23"/>
+      <c r="BJ1" s="23"/>
+      <c r="BK1" s="23">
         <v>43353</v>
       </c>
-      <c r="BL1" s="26"/>
-      <c r="BM1" s="26"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="26"/>
-      <c r="BP1" s="26">
+      <c r="BL1" s="23"/>
+      <c r="BM1" s="23"/>
+      <c r="BN1" s="23"/>
+      <c r="BO1" s="23"/>
+      <c r="BP1" s="23">
         <v>43360</v>
       </c>
-      <c r="BQ1" s="26"/>
-      <c r="BR1" s="26"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26">
+      <c r="BQ1" s="23"/>
+      <c r="BR1" s="23"/>
+      <c r="BS1" s="23"/>
+      <c r="BT1" s="23"/>
+      <c r="BU1" s="23">
         <v>43367</v>
       </c>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26">
+      <c r="BV1" s="23"/>
+      <c r="BW1" s="23"/>
+      <c r="BX1" s="23"/>
+      <c r="BY1" s="23"/>
+      <c r="BZ1" s="23">
         <v>43374</v>
       </c>
-      <c r="CA1" s="26"/>
-      <c r="CB1" s="26"/>
-      <c r="CC1" s="26"/>
-      <c r="CD1" s="26"/>
-      <c r="CE1" s="26">
+      <c r="CA1" s="23"/>
+      <c r="CB1" s="23"/>
+      <c r="CC1" s="23"/>
+      <c r="CD1" s="23"/>
+      <c r="CE1" s="23">
         <v>43381</v>
       </c>
-      <c r="CF1" s="26"/>
-      <c r="CG1" s="26"/>
-      <c r="CH1" s="26"/>
-      <c r="CI1" s="26"/>
-      <c r="CJ1" s="26">
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="23"/>
+      <c r="CI1" s="23"/>
+      <c r="CJ1" s="23">
         <v>43388</v>
       </c>
-      <c r="CK1" s="26"/>
-      <c r="CL1" s="26"/>
-      <c r="CM1" s="26"/>
+      <c r="CK1" s="23"/>
+      <c r="CL1" s="23"/>
+      <c r="CM1" s="23"/>
       <c r="CN1" s="24"/>
-      <c r="CO1" s="26">
+      <c r="CO1" s="23">
         <v>43395</v>
       </c>
-      <c r="CP1" s="26"/>
-      <c r="CQ1" s="26"/>
-      <c r="CR1" s="26"/>
+      <c r="CP1" s="23"/>
+      <c r="CQ1" s="23"/>
+      <c r="CR1" s="23"/>
       <c r="CS1" s="24"/>
     </row>
-    <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="9" t="s">
         <v>3</v>
@@ -1508,7 +1506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1519,7 +1517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1532,7 +1530,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1558,7 +1556,7 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1583,7 +1581,7 @@
       <c r="U6" s="8"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1607,7 +1605,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:98" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1641,7 +1639,7 @@
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
     </row>
-    <row r="9" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:98" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1683,7 +1681,7 @@
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
     </row>
-    <row r="10" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:98" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>22</v>
       </c>
@@ -1728,7 +1726,7 @@
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
     </row>
-    <row r="11" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:98" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1760,7 @@
       <c r="AO11" s="4"/>
       <c r="AS11" s="3"/>
     </row>
-    <row r="12" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1807,7 +1805,7 @@
       <c r="AY12" s="3"/>
       <c r="AZ12" s="3"/>
     </row>
-    <row r="13" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1855,7 +1853,7 @@
       <c r="BG13" s="3"/>
       <c r="BH13" s="3"/>
     </row>
-    <row r="14" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1886,7 +1884,7 @@
       <c r="BQ14" s="3"/>
       <c r="BR14" s="3"/>
     </row>
-    <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>28</v>
       </c>
@@ -1917,7 +1915,7 @@
       <c r="BQ15" s="3"/>
       <c r="BR15" s="3"/>
     </row>
-    <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1953,7 +1951,7 @@
       <c r="BW16" s="3"/>
       <c r="BX16" s="3"/>
     </row>
-    <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1982,7 +1980,7 @@
       <c r="BZ17" s="3"/>
       <c r="CA17" s="3"/>
     </row>
-    <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -2016,7 +2014,7 @@
       <c r="CC18" s="3"/>
       <c r="CD18" s="3"/>
     </row>
-    <row r="19" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -2066,7 +2064,7 @@
       <c r="CO19" s="4"/>
       <c r="CP19" s="4"/>
     </row>
-    <row r="20" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -2074,9 +2072,9 @@
       <c r="CR20" s="3"/>
       <c r="CS20" s="3"/>
     </row>
-    <row r="21" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -2084,19 +2082,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AQ1:AU1"/>
+    <mergeCell ref="AV1:AZ1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
     <mergeCell ref="CE1:CI1"/>
     <mergeCell ref="CJ1:CN1"/>
     <mergeCell ref="CO1:CS1"/>
@@ -2106,15 +2113,6 @@
     <mergeCell ref="BP1:BT1"/>
     <mergeCell ref="BU1:BY1"/>
     <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AQ1:AU1"/>
-    <mergeCell ref="AV1:AZ1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2130,154 +2128,153 @@
       <selection pane="topRight" activeCell="BC20" sqref="BC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" style="2" customWidth="1"/>
-    <col min="2" max="20" width="2.81640625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="2.81640625" style="7" hidden="1" customWidth="1"/>
-    <col min="22" max="44" width="2.81640625" hidden="1" customWidth="1"/>
-    <col min="45" max="47" width="2.7265625" hidden="1" customWidth="1"/>
-    <col min="48" max="97" width="2.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="20" width="2.77734375" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="2.77734375" style="7" hidden="1" customWidth="1"/>
+    <col min="22" max="47" width="2.77734375" hidden="1" customWidth="1"/>
+    <col min="48" max="97" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="26">
+      <c r="B1" s="23">
         <v>43276</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23">
         <v>43283</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23">
         <v>43290</v>
       </c>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26">
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23">
         <v>43297</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
       <c r="U1" s="24"/>
       <c r="V1" s="24">
         <v>43304</v>
       </c>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
       <c r="AA1" s="20"/>
       <c r="AB1" s="21"/>
-      <c r="AC1" s="23">
+      <c r="AC1" s="25">
         <v>43311</v>
       </c>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
       <c r="AH1" s="20"/>
       <c r="AI1" s="21"/>
-      <c r="AJ1" s="23">
+      <c r="AJ1" s="25">
         <v>43318</v>
       </c>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="21"/>
       <c r="AQ1" s="24">
         <v>43325</v>
       </c>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="23">
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="25">
         <v>43332</v>
       </c>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="26">
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="23">
         <v>43339</v>
       </c>
-      <c r="BB1" s="26"/>
-      <c r="BC1" s="26"/>
-      <c r="BD1" s="26"/>
-      <c r="BE1" s="26"/>
-      <c r="BF1" s="26">
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23">
         <v>43346</v>
       </c>
-      <c r="BG1" s="26"/>
-      <c r="BH1" s="26"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="26"/>
-      <c r="BK1" s="26">
+      <c r="BG1" s="23"/>
+      <c r="BH1" s="23"/>
+      <c r="BI1" s="23"/>
+      <c r="BJ1" s="23"/>
+      <c r="BK1" s="23">
         <v>43353</v>
       </c>
-      <c r="BL1" s="26"/>
-      <c r="BM1" s="26"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="26"/>
-      <c r="BP1" s="26">
+      <c r="BL1" s="23"/>
+      <c r="BM1" s="23"/>
+      <c r="BN1" s="23"/>
+      <c r="BO1" s="23"/>
+      <c r="BP1" s="23">
         <v>43360</v>
       </c>
-      <c r="BQ1" s="26"/>
-      <c r="BR1" s="26"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26">
+      <c r="BQ1" s="23"/>
+      <c r="BR1" s="23"/>
+      <c r="BS1" s="23"/>
+      <c r="BT1" s="23"/>
+      <c r="BU1" s="23">
         <v>43367</v>
       </c>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26">
+      <c r="BV1" s="23"/>
+      <c r="BW1" s="23"/>
+      <c r="BX1" s="23"/>
+      <c r="BY1" s="23"/>
+      <c r="BZ1" s="23">
         <v>43374</v>
       </c>
-      <c r="CA1" s="26"/>
-      <c r="CB1" s="26"/>
-      <c r="CC1" s="26"/>
-      <c r="CD1" s="26"/>
-      <c r="CE1" s="26">
+      <c r="CA1" s="23"/>
+      <c r="CB1" s="23"/>
+      <c r="CC1" s="23"/>
+      <c r="CD1" s="23"/>
+      <c r="CE1" s="23">
         <v>43381</v>
       </c>
-      <c r="CF1" s="26"/>
-      <c r="CG1" s="26"/>
-      <c r="CH1" s="26"/>
-      <c r="CI1" s="26"/>
-      <c r="CJ1" s="26">
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="23"/>
+      <c r="CI1" s="23"/>
+      <c r="CJ1" s="23">
         <v>43388</v>
       </c>
-      <c r="CK1" s="26"/>
-      <c r="CL1" s="26"/>
-      <c r="CM1" s="26"/>
+      <c r="CK1" s="23"/>
+      <c r="CL1" s="23"/>
+      <c r="CM1" s="23"/>
       <c r="CN1" s="24"/>
-      <c r="CO1" s="26">
+      <c r="CO1" s="23">
         <v>43395</v>
       </c>
-      <c r="CP1" s="26"/>
-      <c r="CQ1" s="26"/>
-      <c r="CR1" s="26"/>
+      <c r="CP1" s="23"/>
+      <c r="CQ1" s="23"/>
+      <c r="CR1" s="23"/>
       <c r="CS1" s="24"/>
     </row>
-    <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:98" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="9" t="s">
         <v>3</v>
@@ -2571,7 +2568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2582,7 +2579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2595,7 +2592,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2621,7 +2618,7 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2646,7 +2643,7 @@
       <c r="U6" s="8"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:98" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2670,7 +2667,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:98" ht="29.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -2704,7 +2701,7 @@
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
     </row>
-    <row r="9" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:98" ht="29.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2746,7 +2743,7 @@
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
     </row>
-    <row r="10" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:98" ht="29.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>22</v>
       </c>
@@ -2791,7 +2788,7 @@
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
     </row>
-    <row r="11" spans="1:98" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:98" ht="29.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -2825,7 +2822,7 @@
       <c r="AO11" s="4"/>
       <c r="AS11" s="3"/>
     </row>
-    <row r="12" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -2870,7 +2867,7 @@
       <c r="AY12" s="3"/>
       <c r="AZ12" s="3"/>
     </row>
-    <row r="13" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -2898,7 +2895,7 @@
       <c r="BD13" s="3"/>
       <c r="BE13" s="3"/>
     </row>
-    <row r="14" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2926,7 +2923,7 @@
       <c r="BI14" s="3"/>
       <c r="BJ14" s="3"/>
     </row>
-    <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -2957,7 +2954,7 @@
       <c r="BN15" s="3"/>
       <c r="BO15" s="3"/>
     </row>
-    <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:98" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2989,7 +2986,7 @@
       <c r="BS16" s="3"/>
       <c r="BT16" s="3"/>
     </row>
-    <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -3021,7 +3018,7 @@
       <c r="BX17" s="3"/>
       <c r="BY17" s="3"/>
     </row>
-    <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -3071,7 +3068,7 @@
       <c r="CO18" s="4"/>
       <c r="CP18" s="4"/>
     </row>
-    <row r="19" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3079,28 +3076,22 @@
       <c r="CR19" s="3"/>
       <c r="CS19" s="3"/>
     </row>
-    <row r="20" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:97" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
     <mergeCell ref="CO1:CS1"/>
     <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="AQ1:AU1"/>
@@ -3113,6 +3104,12 @@
     <mergeCell ref="BZ1:CD1"/>
     <mergeCell ref="CE1:CI1"/>
     <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>